<commit_message>
qunatified go terms by total spectra
</commit_message>
<xml_diff>
--- a/analyses/metagomics/susvsink/264+265/go_report_264+265_06.28.18.xlsx
+++ b/analyses/metagomics/susvsink/264+265/go_report_264+265_06.28.18.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/metagomics/susvsink/264+265/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{DCE06DDD-456F-6145-9F9B-F55733438035}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3DC414-21C1-5643-AAB9-D8F42C3B3832}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3220" yWindow="3220" windowWidth="27240" windowHeight="16440" activeTab="1"/>
+    <workbookView xWindow="1740" yWindow="3740" windowWidth="27240" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="go_report_264+265_06.28.18" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,12 @@
     <sheet name="molecular function" sheetId="4" r:id="rId4"/>
     <sheet name="compiled" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9561" uniqueCount="3187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9562" uniqueCount="3187">
   <si>
     <t># MetaGOmics GO report</t>
   </si>
@@ -9590,7 +9590,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20">
     <font>
       <sz val="12"/>
@@ -10482,11 +10482,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1593"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="A1:F1593"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -42318,11 +42318,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F1094"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A264" workbookViewId="0">
+      <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -64222,11 +64222,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F245"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I245"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -64237,7 +64237,7 @@
     <col min="7" max="7" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" ht="33" customHeight="1">
+    <row r="1" spans="1:9" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -64257,7 +64257,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>250</v>
       </c>
@@ -64277,7 +64277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -64296,8 +64296,15 @@
       <c r="F3" s="1">
         <v>0.86388385000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="H3" t="s">
+        <v>3054</v>
+      </c>
+      <c r="I3">
+        <f>SUM(D23,D28,D29,D53)</f>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>2036</v>
       </c>
@@ -64317,7 +64324,7 @@
         <v>0.13611614999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>1954</v>
       </c>
@@ -64337,7 +64344,7 @@
         <v>0.11615245</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>1119</v>
       </c>
@@ -64357,7 +64364,7 @@
         <v>9.8003629999999994E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>1121</v>
       </c>
@@ -64377,7 +64384,7 @@
         <v>9.4373869999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>1125</v>
       </c>
@@ -64397,7 +64404,7 @@
         <v>9.0744099999999994E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>437</v>
       </c>
@@ -64417,7 +64424,7 @@
         <v>8.7114339999999998E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>549</v>
       </c>
@@ -64437,7 +64444,7 @@
         <v>8.7114339999999998E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>1139</v>
       </c>
@@ -64457,7 +64464,7 @@
         <v>8.7114339999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>2002</v>
       </c>
@@ -64477,7 +64484,7 @@
         <v>8.5299459999999994E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>2285</v>
       </c>
@@ -64497,7 +64504,7 @@
         <v>8.5299459999999994E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>1948</v>
       </c>
@@ -64517,7 +64524,7 @@
         <v>8.1669690000000003E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>2006</v>
       </c>
@@ -64537,7 +64544,7 @@
         <v>8.1669690000000003E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
         <v>1958</v>
       </c>
@@ -69146,11 +69153,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F253"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -74230,7 +74237,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
running unipept searches on propep list for susvsink
</commit_message>
<xml_diff>
--- a/analyses/metagomics/susvsink/264+265/go_report_264+265_06.28.18.xlsx
+++ b/analyses/metagomics/susvsink/264+265/go_report_264+265_06.28.18.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/metagomics/susvsink/264+265/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3DC414-21C1-5643-AAB9-D8F42C3B3832}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6984D1A-5B77-5D4E-A983-1D0E0A28361E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="3740" windowWidth="27240" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1740" yWindow="460" windowWidth="27240" windowHeight="14720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="go_report_264+265_06.28.18" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9562" uniqueCount="3187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9567" uniqueCount="3189">
   <si>
     <t># MetaGOmics GO report</t>
   </si>
@@ -9585,6 +9585,12 @@
   </si>
   <si>
     <t>contractile ring</t>
+  </si>
+  <si>
+    <t>counts</t>
+  </si>
+  <si>
+    <t>extracellular</t>
   </si>
 </sst>
 </file>
@@ -64226,7 +64232,7 @@
   <dimension ref="A1:I245"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="H3" sqref="H3:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -64296,12 +64302,8 @@
       <c r="F3" s="1">
         <v>0.86388385000000001</v>
       </c>
-      <c r="H3" t="s">
-        <v>3054</v>
-      </c>
-      <c r="I3">
-        <f>SUM(D23,D28,D29,D53)</f>
-        <v>106</v>
+      <c r="I3" t="s">
+        <v>3187</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -64323,6 +64325,13 @@
       <c r="F4" s="1">
         <v>0.13611614999999999</v>
       </c>
+      <c r="H4" t="s">
+        <v>3002</v>
+      </c>
+      <c r="I4">
+        <f>SUM(D12,D17,D20,D59,D141,D189)</f>
+        <v>160</v>
+      </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
@@ -64343,6 +64352,13 @@
       <c r="F5" s="1">
         <v>0.11615245</v>
       </c>
+      <c r="H5" t="s">
+        <v>3054</v>
+      </c>
+      <c r="I5">
+        <f>SUM(D23,D28,D29,D51,D53,D54)</f>
+        <v>148</v>
+      </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
@@ -64363,6 +64379,13 @@
       <c r="F6" s="1">
         <v>9.8003629999999994E-2</v>
       </c>
+      <c r="H6" t="s">
+        <v>2286</v>
+      </c>
+      <c r="I6">
+        <f>SUM(D7,D10,D13,D16,D18,D35,D40,D43,D44,D45,D47,D48,D49,D51,D52,D53,D54,D69,D65,D75,D71,D88,D110,D118,D126,D193,D198,D199,D209,D213,D220,D224,D229,D230,D238,D244)</f>
+        <v>594</v>
+      </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
@@ -64383,6 +64406,13 @@
       <c r="F7" s="1">
         <v>9.4373869999999999E-2</v>
       </c>
+      <c r="H7" t="s">
+        <v>422</v>
+      </c>
+      <c r="I7">
+        <f>SUM(D30,D91)</f>
+        <v>37</v>
+      </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
@@ -64402,6 +64432,13 @@
       </c>
       <c r="F8" s="1">
         <v>9.0744099999999994E-2</v>
+      </c>
+      <c r="H8" t="s">
+        <v>3188</v>
+      </c>
+      <c r="I8">
+        <f>SUM(D63,D64,D65,D66,D67)</f>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:9">

</xml_diff>